<commit_message>
Test scripts added by Harichandana
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/tracker_data.xlsx
+++ b/src/test/resources/testData/tracker_data.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" windowHeight="8016" windowWidth="14808" xWindow="240" yWindow="108"/>
   </bookViews>
   <sheets>
-    <sheet name="Tracker" r:id="rId6" sheetId="1577"/>
+    <sheet name="Tracker" r:id="rId6" sheetId="1585"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -5676,7 +5676,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1577.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1585.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Test scripts added by Bhavya
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/tracker_data.xlsx
+++ b/src/test/resources/testData/tracker_data.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" windowHeight="8016" windowWidth="14808" xWindow="240" yWindow="108"/>
   </bookViews>
   <sheets>
-    <sheet name="Tracker" r:id="rId6" sheetId="1585"/>
+    <sheet name="Tracker" r:id="rId6" sheetId="1589"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -5676,7 +5676,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1585.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1589.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>